<commit_message>
Revise RTED example case
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_rted.xlsx
+++ b/ams/cases/ieee14/ieee14_rted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jwang\work\ams\ams\cases\ieee14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550993E4-72A9-4D5D-9E59-200BA1B3CA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B19C53A-27B6-7347-98BA-864F93B15FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="Area" sheetId="7" r:id="rId7"/>
     <sheet name="GCost" sheetId="8" r:id="rId8"/>
     <sheet name="RCost" sheetId="9" r:id="rId9"/>
+    <sheet name="Zone" sheetId="10" r:id="rId10"/>
+    <sheet name="AGCR" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="256">
   <si>
     <t>uid</t>
   </si>
@@ -763,10 +765,6 @@
   </si>
   <si>
     <t>rate_a</t>
-  </si>
-  <si>
-    <t>cr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>RCOST_1</t>
@@ -783,6 +781,24 @@
   </si>
   <si>
     <t>RCOST_5</t>
+  </si>
+  <si>
+    <t>cru</t>
+  </si>
+  <si>
+    <t>crd</t>
+  </si>
+  <si>
+    <t>ZONE1</t>
+  </si>
+  <si>
+    <t>ZONE2</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>dd</t>
   </si>
 </sst>
 </file>
@@ -793,13 +809,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -825,8 +841,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1169,12 +1188,12 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1256,13 +1275,13 @@
         <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1300,13 +1319,13 @@
         <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="N3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1344,13 +1363,13 @@
         <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="N4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1388,13 +1407,13 @@
         <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="N5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1432,13 +1451,13 @@
         <v>15</v>
       </c>
       <c r="M6" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="N6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1476,13 +1495,13 @@
         <v>21</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1520,13 +1539,13 @@
         <v>21</v>
       </c>
       <c r="M8" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1564,13 +1583,13 @@
         <v>21</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1608,13 +1627,13 @@
         <v>21</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1652,13 +1671,13 @@
         <v>21</v>
       </c>
       <c r="M11" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1696,13 +1715,13 @@
         <v>21</v>
       </c>
       <c r="M12" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1740,13 +1759,13 @@
         <v>21</v>
       </c>
       <c r="M13" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1784,13 +1803,13 @@
         <v>21</v>
       </c>
       <c r="M14" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1828,7 +1847,7 @@
         <v>21</v>
       </c>
       <c r="M15" t="s">
-        <v>21</v>
+        <v>253</v>
       </c>
       <c r="N15" t="s">
         <v>21</v>
@@ -1839,8 +1858,140 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:N15" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:N1 A8:L15 A2:L2 N2 A3:L3 N3 A4:L6 N4:N6 A7:L7 N7 N8:N15" numberStoredAsText="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D304DCD5-B58C-2F40-B69E-C9870B13ADFC}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC1EB84-6F53-6A4C-A2DF-7A3636DD1DD1}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1850,9 +2001,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +2062,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1967,7 +2118,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2023,7 +2174,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2079,7 +2230,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2150,9 +2301,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2214,7 +2365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2288,9 +2439,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2325,7 +2476,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2360,7 +2511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2395,7 +2546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2430,7 +2581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2465,7 +2616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2500,7 +2651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2535,7 +2686,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2570,7 +2721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2605,7 +2756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2640,7 +2791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2675,7 +2826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2727,9 +2878,9 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +2957,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2874,7 +3025,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2942,7 +3093,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3010,7 +3161,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3078,7 +3229,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3146,7 +3297,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3214,7 +3365,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3282,7 +3433,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -3350,7 +3501,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3418,7 +3569,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3486,7 +3637,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -3554,7 +3705,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -3622,7 +3773,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3690,7 +3841,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3758,7 +3909,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3826,7 +3977,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>206</v>
       </c>
@@ -3894,7 +4045,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>210</v>
       </c>
@@ -3962,7 +4113,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -4030,7 +4181,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>217</v>
       </c>
@@ -4098,7 +4249,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>220</v>
       </c>
@@ -4181,9 +4332,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4215,7 +4366,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4247,7 +4398,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4292,11 +4443,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="A1:D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4310,7 +4463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4324,7 +4477,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4355,9 +4508,9 @@
       <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4386,7 +4539,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4415,7 +4568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4444,7 +4597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4473,7 +4626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4502,7 +4655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -4542,15 +4695,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B97D1-6F67-409E-B307-E3878FB294FD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4561,15 +4714,18 @@
         <v>228</v>
       </c>
       <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>246</v>
       </c>
       <c r="C2" t="s">
         <v>104</v>
@@ -4577,13 +4733,16 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>
@@ -4591,13 +4750,16 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
         <v>95</v>
@@ -4605,13 +4767,16 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C5" t="s">
         <v>98</v>
@@ -4619,18 +4784,24 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C6" t="s">
         <v>102</v>
       </c>
       <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename AGCR to SFR, rename RCost to SFRCost
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_rted.xlsx
+++ b/ams/cases/ieee14/ieee14_rted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jwang\work\ams\ams\cases\ieee14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D6403D-E9D3-9243-8192-10D163C8879C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A9BE4-3CE4-46CE-BF32-4F1F277CA046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="Shunt" sheetId="6" r:id="rId6"/>
     <sheet name="Area" sheetId="7" r:id="rId7"/>
     <sheet name="GCost" sheetId="8" r:id="rId8"/>
-    <sheet name="RCost" sheetId="9" r:id="rId9"/>
-    <sheet name="Zone" sheetId="10" r:id="rId10"/>
-    <sheet name="AGCR" sheetId="11" r:id="rId11"/>
+    <sheet name="Zone" sheetId="10" r:id="rId9"/>
+    <sheet name="SFR" sheetId="11" r:id="rId10"/>
+    <sheet name="SFRCost" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -815,13 +815,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1193,13 +1193,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1870,63 +1870,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D304DCD5-B58C-2F40-B69E-C9870B13ADFC}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC1EB84-6F53-6A4C-A2DF-7A3636DD1DD1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1934,9 +1877,9 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1959,7 +1902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1982,7 +1925,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2006,6 +1949,125 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B97D1-6F67-409E-B307-E3878FB294FD}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2016,9 +2078,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2133,7 +2195,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2189,7 +2251,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2245,7 +2307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2316,9 +2378,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2454,9 +2516,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2526,7 +2588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2561,7 +2623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2596,7 +2658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2631,7 +2693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2666,7 +2728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2701,7 +2763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2736,7 +2798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2771,7 +2833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2806,7 +2868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2841,7 +2903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2893,9 +2955,9 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2972,7 +3034,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3040,7 +3102,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3108,7 +3170,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3176,7 +3238,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3244,7 +3306,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3312,7 +3374,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3380,7 +3442,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3448,7 +3510,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -3516,7 +3578,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3584,7 +3646,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3652,7 +3714,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -3720,7 +3782,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -3788,7 +3850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3856,7 +3918,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3924,7 +3986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -3992,7 +4054,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>206</v>
       </c>
@@ -4060,7 +4122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>210</v>
       </c>
@@ -4128,7 +4190,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -4196,7 +4258,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>217</v>
       </c>
@@ -4264,7 +4326,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>220</v>
       </c>
@@ -4347,9 +4409,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4381,7 +4443,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4413,7 +4475,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4462,9 +4524,9 @@
       <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4478,7 +4540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4492,7 +4554,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4523,9 +4585,9 @@
       <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4554,7 +4616,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4583,7 +4645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4612,7 +4674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4641,7 +4703,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4670,7 +4732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -4709,16 +4771,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B97D1-6F67-409E-B307-E3878FB294FD}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D304DCD5-B58C-2F40-B69E-C9870B13ADFC}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4726,102 +4788,43 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>246</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>249</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rename model Zone to Region
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_rted.xlsx
+++ b/ams/cases/ieee14/ieee14_rted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jwang\work\ams\ams\cases\ieee14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A9BE4-3CE4-46CE-BF32-4F1F277CA046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B01FC84-6D58-C943-AF4C-442538B15BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Shunt" sheetId="6" r:id="rId6"/>
     <sheet name="Area" sheetId="7" r:id="rId7"/>
     <sheet name="GCost" sheetId="8" r:id="rId8"/>
-    <sheet name="Zone" sheetId="10" r:id="rId9"/>
+    <sheet name="Region" sheetId="10" r:id="rId9"/>
     <sheet name="SFR" sheetId="11" r:id="rId10"/>
     <sheet name="SFRCost" sheetId="9" r:id="rId11"/>
   </sheets>
@@ -815,13 +815,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1197,9 +1197,9 @@
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1877,9 +1877,9 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1958,13 +1958,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B97D1-6F67-409E-B307-E3878FB294FD}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2078,9 +2078,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2378,9 +2378,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2516,9 +2516,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2955,9 +2955,9 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>206</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>210</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>217</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>220</v>
       </c>
@@ -4409,9 +4409,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4524,9 +4524,9 @@
       <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4585,9 +4585,9 @@
       <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -4774,13 +4774,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D304DCD5-B58C-2F40-B69E-C9870B13ADFC}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>

</xml_diff>